<commit_message>
Add Log Log Plot
</commit_message>
<xml_diff>
--- a/Project 1 Experimental Analysis.xlsx
+++ b/Project 1 Experimental Analysis.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\__CS325 - Analysis of Algorithms\project 1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-60" yWindow="60" windowWidth="18405" windowHeight="10995"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Input Size</t>
   </si>
@@ -34,14 +29,33 @@
   <si>
     <t>Project Group: Darnel Clayton, Rudy Gonzalez, Brad Parker</t>
   </si>
+  <si>
+    <t>Log - Log Plot</t>
+  </si>
+  <si>
+    <t>Algorithm 1 Time</t>
+  </si>
+  <si>
+    <t>Algorithm 2 Time</t>
+  </si>
+  <si>
+    <t>Algorithm 3 Time</t>
+  </si>
+  <si>
+    <t>Algorithm 4 Time</t>
+  </si>
+  <si>
+    <t>Size(n)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -155,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -184,6 +198,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -265,23 +283,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -427,11 +428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1529089744"/>
-        <c:axId val="1529089200"/>
+        <c:axId val="39743488"/>
+        <c:axId val="39745024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1529089744"/>
+        <c:axId val="39743488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -484,23 +485,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -535,12 +519,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1529089200"/>
+        <c:crossAx val="39745024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1529089200"/>
+        <c:axId val="39745024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,23 +575,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -637,7 +604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1529089744"/>
+        <c:crossAx val="39743488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -747,23 +714,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -906,11 +856,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1648447856"/>
-        <c:axId val="1648444592"/>
+        <c:axId val="145242368"/>
+        <c:axId val="145252736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1648447856"/>
+        <c:axId val="145242368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -963,23 +913,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1014,12 +947,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1648444592"/>
+        <c:crossAx val="145252736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1648444592"/>
+        <c:axId val="145252736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1072,23 +1005,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -1118,7 +1034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1648447856"/>
+        <c:crossAx val="145242368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1232,23 +1148,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1407,11 +1306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1649877968"/>
-        <c:axId val="1649876336"/>
+        <c:axId val="40527744"/>
+        <c:axId val="40538112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1649877968"/>
+        <c:axId val="40527744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000"/>
@@ -1464,23 +1363,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1515,12 +1397,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1649876336"/>
+        <c:crossAx val="40538112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1649876336"/>
+        <c:axId val="40538112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -1572,23 +1454,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -1618,7 +1483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1649877968"/>
+        <c:crossAx val="40527744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1720,23 +1585,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1878,11 +1726,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1649875792"/>
-        <c:axId val="1649875248"/>
+        <c:axId val="40909056"/>
+        <c:axId val="40911232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1649875792"/>
+        <c:axId val="40909056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -1935,23 +1783,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1986,12 +1817,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1649875248"/>
+        <c:crossAx val="40911232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1649875248"/>
+        <c:axId val="40911232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -2043,23 +1874,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -2089,7 +1903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1649875792"/>
+        <c:crossAx val="40909056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2131,6 +1945,822 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="portrait" verticalDpi="0"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="107"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="7"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Log-Log Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9822495362053467E-2"/>
+          <c:y val="1.01275246416122E-2"/>
+          <c:w val="0.76030309298666787"/>
+          <c:h val="0.92184290587149298"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$184</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dot"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$185:$B$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$185:$C$212</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>2.9040408134460401E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21246006488800001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70382559299468905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7121263504028299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.41208438873291</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9285577535629201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5556417942047105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.3401399135589</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.328822016716</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.081754541397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$184</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 2 Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$185:$B$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$185:$D$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="9" formatCode="0.0000000">
+                  <c:v>0.14980137348174999</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0000000">
+                  <c:v>0.59123957157134999</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.0000000">
+                  <c:v>1.3631712436676</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.0000000">
+                  <c:v>2.3918435811996401</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0000000">
+                  <c:v>3.78381640911102</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.0000000">
+                  <c:v>5.3925208806991503</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.0000000">
+                  <c:v>7.2912087202072096</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.0000000">
+                  <c:v>9.5153646230697593</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.0000000">
+                  <c:v>12.1277544260025</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.0000000">
+                  <c:v>14.9287435293197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$184</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 3 Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$185:$B$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$185:$E$212</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>0.63696053028106603</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>1.30299079418182</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>1.9801072359084999</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>2.6483353137969901</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>3.3874741315841601</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>4.0416463613510096</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>4.7328126192092803</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>5.4139649868011404</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>6.1112284183502199</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>6.8721181631088202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$184</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 4 Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$185:$B$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$185:$F$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="18" formatCode="0.0000000">
+                  <c:v>0.25738258361816402</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.0000000">
+                  <c:v>0.53304800987243595</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.0000000">
+                  <c:v>0.805363392829895</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.0000000">
+                  <c:v>1.0600845098495399</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.0000000">
+                  <c:v>1.2999391317367499</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.0000000">
+                  <c:v>1.5357988119125301</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.0000000">
+                  <c:v>1.8676990985870301</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.0000000">
+                  <c:v>2.0316090345382598</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.0000000">
+                  <c:v>2.41001198291778</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.0000000">
+                  <c:v>2.7088038444519</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="56706944"/>
+        <c:axId val="56705408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="56706944"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56705408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="56705408"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56706944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84395879323991974"/>
+          <c:y val="0.75687898327805236"/>
+          <c:w val="0.12403761506786962"/>
+          <c:h val="0.13351476142941773"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4563,6 +5193,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>84665</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>30688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243417</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4609,7 +5269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4644,7 +5304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4853,22 +5513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K181"/>
+  <dimension ref="A1:K230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A171" sqref="A171"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J178" sqref="J178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
@@ -5600,7 +6251,7 @@
         <v>1.2999391317367499</v>
       </c>
     </row>
-    <row r="177" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C177" s="11">
         <v>6000000</v>
       </c>
@@ -5608,7 +6259,7 @@
         <v>1.5357988119125301</v>
       </c>
     </row>
-    <row r="178" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C178" s="11">
         <v>7000000</v>
       </c>
@@ -5616,7 +6267,7 @@
         <v>1.8676990985870301</v>
       </c>
     </row>
-    <row r="179" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C179" s="11">
         <v>8000000</v>
       </c>
@@ -5624,7 +6275,7 @@
         <v>2.0316090345382598</v>
       </c>
     </row>
-    <row r="180" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C180" s="11">
         <v>9000000</v>
       </c>
@@ -5632,13 +6283,372 @@
         <v>2.41001198291778</v>
       </c>
     </row>
-    <row r="181" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C181" s="11">
         <v>10000000</v>
       </c>
       <c r="D181" s="13">
         <v>2.7088038444519</v>
       </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D184" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F184" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G184" s="15"/>
+      <c r="H184" s="15"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>100</v>
+      </c>
+      <c r="C185" s="14">
+        <v>2.9040408134460401E-2</v>
+      </c>
+      <c r="E185" s="14"/>
+      <c r="G185" s="14"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>200</v>
+      </c>
+      <c r="C186" s="14">
+        <v>0.21246006488800001</v>
+      </c>
+      <c r="E186" s="14"/>
+      <c r="G186" s="14"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>300</v>
+      </c>
+      <c r="C187" s="14">
+        <v>0.70382559299468905</v>
+      </c>
+      <c r="E187" s="14"/>
+      <c r="G187" s="14"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>400</v>
+      </c>
+      <c r="C188" s="14">
+        <v>1.7121263504028299</v>
+      </c>
+      <c r="E188" s="14"/>
+      <c r="G188" s="14"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>500</v>
+      </c>
+      <c r="C189" s="14">
+        <v>3.41208438873291</v>
+      </c>
+      <c r="E189" s="14"/>
+      <c r="G189" s="14"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>600</v>
+      </c>
+      <c r="C190" s="14">
+        <v>5.9285577535629201</v>
+      </c>
+      <c r="E190" s="14"/>
+      <c r="G190" s="14"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>700</v>
+      </c>
+      <c r="C191" s="14">
+        <v>9.5556417942047105</v>
+      </c>
+      <c r="E191" s="14"/>
+      <c r="G191" s="14"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>800</v>
+      </c>
+      <c r="C192" s="14">
+        <v>14.3401399135589</v>
+      </c>
+      <c r="E192" s="14"/>
+      <c r="G192" s="14"/>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>900</v>
+      </c>
+      <c r="C193" s="14">
+        <v>20.328822016716</v>
+      </c>
+      <c r="E193" s="14"/>
+      <c r="G193" s="14"/>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>1000</v>
+      </c>
+      <c r="C194" s="14">
+        <v>28.081754541397</v>
+      </c>
+      <c r="D194" s="14">
+        <v>0.14980137348174999</v>
+      </c>
+      <c r="E194" s="14"/>
+      <c r="G194" s="14"/>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>2000</v>
+      </c>
+      <c r="D195" s="14">
+        <v>0.59123957157134999</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>3000</v>
+      </c>
+      <c r="D196" s="14">
+        <v>1.3631712436676</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>4000</v>
+      </c>
+      <c r="D197" s="14">
+        <v>2.3918435811996401</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>5000</v>
+      </c>
+      <c r="D198" s="14">
+        <v>3.78381640911102</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>6000</v>
+      </c>
+      <c r="D199" s="14">
+        <v>5.3925208806991503</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>7000</v>
+      </c>
+      <c r="D200" s="14">
+        <v>7.2912087202072096</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>8000</v>
+      </c>
+      <c r="D201" s="14">
+        <v>9.5153646230697593</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>9000</v>
+      </c>
+      <c r="D202" s="14">
+        <v>12.1277544260025</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>10000</v>
+      </c>
+      <c r="D203" s="14">
+        <v>14.9287435293197</v>
+      </c>
+      <c r="E203">
+        <v>0.63696053028106603</v>
+      </c>
+      <c r="F203" s="14">
+        <v>0.25738258361816402</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>200000</v>
+      </c>
+      <c r="E204">
+        <v>1.30299079418182</v>
+      </c>
+      <c r="F204" s="14">
+        <v>0.53304800987243595</v>
+      </c>
+    </row>
+    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>300000</v>
+      </c>
+      <c r="E205">
+        <v>1.9801072359084999</v>
+      </c>
+      <c r="F205" s="14">
+        <v>0.805363392829895</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>400000</v>
+      </c>
+      <c r="E206">
+        <v>2.6483353137969901</v>
+      </c>
+      <c r="F206" s="14">
+        <v>1.0600845098495399</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>500000</v>
+      </c>
+      <c r="E207">
+        <v>3.3874741315841601</v>
+      </c>
+      <c r="F207" s="14">
+        <v>1.2999391317367499</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>600000</v>
+      </c>
+      <c r="C208" s="15"/>
+      <c r="E208">
+        <v>4.0416463613510096</v>
+      </c>
+      <c r="F208" s="14">
+        <v>1.5357988119125301</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>700000</v>
+      </c>
+      <c r="C209" s="14"/>
+      <c r="E209">
+        <v>4.7328126192092803</v>
+      </c>
+      <c r="F209" s="14">
+        <v>1.8676990985870301</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>800000</v>
+      </c>
+      <c r="C210" s="14"/>
+      <c r="E210">
+        <v>5.4139649868011404</v>
+      </c>
+      <c r="F210" s="14">
+        <v>2.0316090345382598</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>900000</v>
+      </c>
+      <c r="C211" s="14"/>
+      <c r="E211">
+        <v>6.1112284183502199</v>
+      </c>
+      <c r="F211" s="14">
+        <v>2.41001198291778</v>
+      </c>
+    </row>
+    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>1000000</v>
+      </c>
+      <c r="C212" s="14"/>
+      <c r="E212">
+        <v>6.8721181631088202</v>
+      </c>
+      <c r="F212" s="14">
+        <v>2.7088038444519</v>
+      </c>
+    </row>
+    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C213" s="14"/>
+    </row>
+    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C214" s="14"/>
+    </row>
+    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C215" s="14"/>
+    </row>
+    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C216" s="14"/>
+    </row>
+    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C217" s="14"/>
+    </row>
+    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C218" s="14"/>
+    </row>
+    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B220" s="15"/>
+      <c r="C220" s="15"/>
+    </row>
+    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C221" s="14"/>
+    </row>
+    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C222" s="14"/>
+    </row>
+    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C223" s="14"/>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C224" s="14"/>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C225" s="14"/>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C226" s="14"/>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C227" s="14"/>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C228" s="14"/>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C229" s="14"/>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C230" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding second log-log plot to correct starting n value errors for algs 3 and 4 in first plot. Formatted to match other graphs.
</commit_message>
<xml_diff>
--- a/Project 1 Experimental Analysis.xlsx
+++ b/Project 1 Experimental Analysis.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\GitHub\cs325\CS325_Analysis_of_Algorithms\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-60" yWindow="60" windowWidth="18405" windowHeight="10995"/>
   </bookViews>
@@ -55,7 +60,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -198,7 +203,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -283,6 +288,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -337,8 +359,41 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.47247936092394804"/>
+                  <c:y val="1.5283662854149904E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -428,11 +483,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="39743488"/>
-        <c:axId val="39745024"/>
+        <c:axId val="-349421024"/>
+        <c:axId val="-349424832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39743488"/>
+        <c:axId val="-349421024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -485,6 +540,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -519,12 +591,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39745024"/>
+        <c:crossAx val="-349424832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39745024"/>
+        <c:axId val="-349424832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,6 +647,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -604,7 +693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39743488"/>
+        <c:crossAx val="-349421024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -714,6 +803,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -765,8 +871,41 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.55498781413268727"/>
+                  <c:y val="4.5319762571090133E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -856,11 +995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145242368"/>
-        <c:axId val="145252736"/>
+        <c:axId val="-349429184"/>
+        <c:axId val="-349430816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145242368"/>
+        <c:axId val="-349429184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -913,6 +1052,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -947,12 +1103,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145252736"/>
+        <c:crossAx val="-349430816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145252736"/>
+        <c:axId val="-349430816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1005,6 +1161,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -1034,7 +1207,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145242368"/>
+        <c:crossAx val="-349429184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1148,6 +1321,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1197,26 +1387,42 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:alpha val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.63492536366759245"/>
+                  <c:y val="2.1903248101276415E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1306,11 +1512,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40527744"/>
-        <c:axId val="40538112"/>
+        <c:axId val="-349430272"/>
+        <c:axId val="-349425920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40527744"/>
+        <c:axId val="-349430272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000"/>
@@ -1363,6 +1569,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1397,12 +1620,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40538112"/>
+        <c:crossAx val="-349425920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40538112"/>
+        <c:axId val="-349425920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -1454,6 +1677,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -1483,7 +1723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40527744"/>
+        <c:crossAx val="-349430272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1585,6 +1825,23 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1635,8 +1892,41 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.63530410221983735"/>
+                  <c:y val="-1.7138041802755424E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1726,11 +2016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40909056"/>
-        <c:axId val="40911232"/>
+        <c:axId val="-349429728"/>
+        <c:axId val="-349428640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40909056"/>
+        <c:axId val="-349429728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -1769,7 +2059,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Size</a:t>
+                  <a:t>size</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1783,6 +2073,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1817,12 +2124,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40911232"/>
+        <c:crossAx val="-349428640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40911232"/>
+        <c:axId val="-349428640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -1874,6 +2181,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -1903,7 +2227,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40909056"/>
+        <c:crossAx val="-349429728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1944,7 +2268,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup orientation="portrait" verticalDpi="0"/>
+    <c:pageSetup orientation="portrait" verticalDpi="-3"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2659,11 +2983,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56706944"/>
-        <c:axId val="56705408"/>
+        <c:axId val="-349419392"/>
+        <c:axId val="-349427552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56706944"/>
+        <c:axId val="-349419392"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2698,12 +3022,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56705408"/>
+        <c:crossAx val="-349427552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56705408"/>
+        <c:axId val="-349427552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2734,7 +3058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56706944"/>
+        <c:crossAx val="-349419392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2761,6 +3085,907 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>log-log plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>algorithm 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$35:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$35:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.9040408134460401E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21246006488800001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70382559299468905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7121263504028299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.41208438873291</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9285577535629201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5556417942047105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.3401399135589</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.328822016716</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.081754541397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>algorithm 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent2"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$80:$C$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$80:$D$89</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.14980137348174999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59123957157134999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3631712436676</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3918435811996401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.78381640911102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3925208806991503</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.2912087202072096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5153646230697593</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.1277544260025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.9287435293197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>algorithm 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent3"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FFFF00">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$126:$C$135</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$126:$D$135</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.63696053028106603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.30299079418182</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9801072359084999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6483353137969901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3874741315841601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0416463613510096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7328126192092803</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4139649868011404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1112284183502199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8721181631088202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>algorithm 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent4"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="00B050">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$172:$C$181</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$172:$D$181</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.25738258361816402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53304800987243595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.805363392829895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0600845098495399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2999391317367499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5357988119125301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8676990985870301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0316090345382598</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.41001198291778</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.7088038444519</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-148890288"/>
+        <c:axId val="-148883216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-148890288"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-148883216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-148883216"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-148890288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait" verticalDpi="-3"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2925,6 +4150,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
   <cs:axisTitle>
@@ -4531,6 +5796,541 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5223,6 +7023,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>223</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>395288</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5269,7 +7101,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5304,7 +7136,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5515,8 +7347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J178" sqref="J178"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated log-log plot and program code
</commit_message>
<xml_diff>
--- a/Project 1 Experimental Analysis.xlsx
+++ b/Project 1 Experimental Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\GitHub\cs325\CS325_Analysis_of_Algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\__CS325 - Analysis of Algorithms\project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Input Size</t>
   </si>
@@ -52,6 +52,24 @@
   <si>
     <t>Size(n)</t>
   </si>
+  <si>
+    <t>Avg Times</t>
+  </si>
+  <si>
+    <t>Algorithm 1</t>
+  </si>
+  <si>
+    <t>Algorithm 2</t>
+  </si>
+  <si>
+    <t>Algorithm 3</t>
+  </si>
+  <si>
+    <t>Algorithm 4</t>
+  </si>
+  <si>
+    <t>Data Logartihm Tables</t>
+  </si>
 </sst>
 </file>
 
@@ -62,7 +80,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +143,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -170,11 +195,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -207,6 +241,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,11 +524,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-349421024"/>
-        <c:axId val="-349424832"/>
+        <c:axId val="241343216"/>
+        <c:axId val="241349744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-349421024"/>
+        <c:axId val="241343216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -591,12 +632,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349424832"/>
+        <c:crossAx val="241349744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-349424832"/>
+        <c:axId val="241349744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,7 +734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349421024"/>
+        <c:crossAx val="241343216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -995,11 +1036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-349429184"/>
-        <c:axId val="-349430816"/>
+        <c:axId val="241353008"/>
+        <c:axId val="241351920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-349429184"/>
+        <c:axId val="241353008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -1103,12 +1144,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349430816"/>
+        <c:crossAx val="241351920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-349430816"/>
+        <c:axId val="241351920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1207,7 +1248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349429184"/>
+        <c:crossAx val="241353008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1424,6 +1465,22 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$126:$C$135</c:f>
@@ -1512,11 +1569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-349430272"/>
-        <c:axId val="-349425920"/>
+        <c:axId val="241350288"/>
+        <c:axId val="241346480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-349430272"/>
+        <c:axId val="241350288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000000"/>
@@ -1620,12 +1677,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349425920"/>
+        <c:crossAx val="241346480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-349425920"/>
+        <c:axId val="241346480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7"/>
@@ -1723,7 +1780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349430272"/>
+        <c:crossAx val="241350288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2016,11 +2073,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-349429728"/>
-        <c:axId val="-349428640"/>
+        <c:axId val="239472736"/>
+        <c:axId val="414904640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-349429728"/>
+        <c:axId val="239472736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -2124,12 +2181,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349428640"/>
+        <c:crossAx val="414904640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-349428640"/>
+        <c:axId val="414904640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -2227,7 +2284,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-349429728"/>
+        <c:crossAx val="239472736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2983,11 +3040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-349419392"/>
-        <c:axId val="-349427552"/>
+        <c:axId val="414914432"/>
+        <c:axId val="414910080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-349419392"/>
+        <c:axId val="414914432"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3022,12 +3079,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-349427552"/>
+        <c:crossAx val="414910080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-349427552"/>
+        <c:axId val="414910080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3058,7 +3115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-349419392"/>
+        <c:crossAx val="414914432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3207,7 +3264,35 @@
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3338,7 +3423,35 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3467,7 +3580,35 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3596,7 +3737,35 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3686,11 +3855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-148890288"/>
-        <c:axId val="-148883216"/>
+        <c:axId val="414908992"/>
+        <c:axId val="414909536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-148890288"/>
+        <c:axId val="414908992"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3795,12 +3964,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148883216"/>
+        <c:crossAx val="414909536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-148883216"/>
+        <c:axId val="414909536"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3899,7 +4068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148890288"/>
+        <c:crossAx val="414908992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7345,10 +7514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K230"/>
+  <dimension ref="A1:K281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80:D89"/>
+    <sheetView tabSelected="1" topLeftCell="A213" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D272" sqref="D272:D281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8482,7 +8651,429 @@
     <row r="230" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C230" s="14"/>
     </row>
+    <row r="255" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B255" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C255" s="17"/>
+      <c r="D255" s="17"/>
+    </row>
+    <row r="257" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A257" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B257" s="16"/>
+      <c r="D257" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E257" s="16"/>
+    </row>
+    <row r="258" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A258" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B258" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D258" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E258" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A259" s="18">
+        <f>LOG(100,10)</f>
+        <v>2</v>
+      </c>
+      <c r="B259" s="12">
+        <f>LOG(0.0290404081344604, 10)</f>
+        <v>-1.5369972843459629</v>
+      </c>
+      <c r="D259" s="18">
+        <f>LOG(1000,10)</f>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="E259" s="12">
+        <f>LOG(0.14980137348175, 10)</f>
+        <v>-0.82448420470857853</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A260" s="18">
+        <f>LOG(200,10)</f>
+        <v>2.3010299956639808</v>
+      </c>
+      <c r="B260" s="12">
+        <f>LOG(0.212460064888, 10)</f>
+        <v>-0.67272269021917885</v>
+      </c>
+      <c r="D260" s="18">
+        <f>LOG(2000,10)</f>
+        <v>3.3010299956639808</v>
+      </c>
+      <c r="E260" s="12">
+        <f>LOG(0.59123957157135, 10)</f>
+        <v>-0.22823650637922166</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A261" s="18">
+        <f>LOG(300,10)</f>
+        <v>2.4771212547196622</v>
+      </c>
+      <c r="B261" s="12">
+        <f>LOG(0.703825592994689, 10)</f>
+        <v>-0.1525349450963335</v>
+      </c>
+      <c r="D261" s="18">
+        <f>LOG(3000,10)</f>
+        <v>3.4771212547196617</v>
+      </c>
+      <c r="E261" s="12">
+        <f>LOG(1.3631712436676, 10)</f>
+        <v>0.13455041600228598</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A262" s="18">
+        <f>LOG(400,10)</f>
+        <v>2.6020599913279621</v>
+      </c>
+      <c r="B262" s="12">
+        <f>LOG(1.71212635040283, 10)</f>
+        <v>0.23353581130955364</v>
+      </c>
+      <c r="D262" s="18">
+        <f>LOG(4000,10)</f>
+        <v>3.6020599913279621</v>
+      </c>
+      <c r="E262" s="12">
+        <f>LOG(2.39184358119964, 10)</f>
+        <v>0.37873277479669343</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A263" s="18">
+        <f>LOG(500,10)</f>
+        <v>2.6989700043360183</v>
+      </c>
+      <c r="B263" s="12">
+        <f>LOG(3.41208438873291, 10)</f>
+        <v>0.53301976373458837</v>
+      </c>
+      <c r="D263" s="18">
+        <f>LOG(5000,10)</f>
+        <v>3.6989700043360187</v>
+      </c>
+      <c r="E263" s="12">
+        <f>LOG(3.78381640911102, 10)</f>
+        <v>0.57793005625927618</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A264" s="18">
+        <f>LOG(600,10)</f>
+        <v>2.7781512503836434</v>
+      </c>
+      <c r="B264" s="12">
+        <f>LOG(5.92855775356292, 10)</f>
+        <v>0.77294905494089372</v>
+      </c>
+      <c r="D264" s="18">
+        <f>LOG(6000,10)</f>
+        <v>3.778151250383643</v>
+      </c>
+      <c r="E264" s="12">
+        <f>LOG(5.39252088069915)</f>
+        <v>0.73179183543519688</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A265" s="18">
+        <f>LOG(700,10)</f>
+        <v>2.8450980400142565</v>
+      </c>
+      <c r="B265" s="12">
+        <f>LOG(9.55564179420471, 10)</f>
+        <v>0.98025986128335951</v>
+      </c>
+      <c r="D265" s="18">
+        <f>LOG(7000,10)</f>
+        <v>3.8450980400142565</v>
+      </c>
+      <c r="E265" s="12">
+        <f>LOG(7.29120872020721, 10)</f>
+        <v>0.86279953065021342</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A266" s="18">
+        <f>LOG(800,10)</f>
+        <v>2.9030899869919433</v>
+      </c>
+      <c r="B266" s="12">
+        <f>LOG(14.3401399135589, 10)</f>
+        <v>1.1565533886672166</v>
+      </c>
+      <c r="D266" s="18">
+        <f>LOG(8000,10)</f>
+        <v>3.9030899869919433</v>
+      </c>
+      <c r="E266" s="12">
+        <f>LOG(9.51536462306976, 10)</f>
+        <v>0.97842543484617328</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A267" s="18">
+        <f>LOG(900,10)</f>
+        <v>2.9542425094393248</v>
+      </c>
+      <c r="B267" s="12">
+        <f>LOG(20.328822016716, 10)</f>
+        <v>1.3081122135390619</v>
+      </c>
+      <c r="D267" s="18">
+        <f>LOG(9000,10)</f>
+        <v>3.9542425094393248</v>
+      </c>
+      <c r="E267" s="12">
+        <f>LOG(12.1277544260025, 10)</f>
+        <v>1.0837803943803435</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A268" s="18">
+        <f>LOG(1000,10)</f>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="B268" s="13">
+        <f>LOG(28.081754541397, 10)</f>
+        <v>1.4484242389222295</v>
+      </c>
+      <c r="D268" s="18">
+        <f>LOG(10000,10)</f>
+        <v>4</v>
+      </c>
+      <c r="E268" s="13">
+        <f>LOG(14.9287435293197, 10)</f>
+        <v>1.1740232570722549</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A270" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B270" s="16"/>
+      <c r="D270" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E270" s="16"/>
+    </row>
+    <row r="271" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A271" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B271" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D271" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E271" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A272" s="18">
+        <f>LOG(100000, 10)</f>
+        <v>5</v>
+      </c>
+      <c r="B272" s="12">
+        <f>LOG(0.636960530281066, 10)</f>
+        <v>-0.19588747820188102</v>
+      </c>
+      <c r="D272" s="18">
+        <f>LOG(1000000, 10)</f>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="E272" s="12">
+        <f>LOG(0.257382583618164, 10)</f>
+        <v>-0.58942084396788896</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A273" s="18">
+        <f>LOG(200000, 10)</f>
+        <v>5.3010299956639813</v>
+      </c>
+      <c r="B273" s="12">
+        <f>LOG(1.30299079418182, 10)</f>
+        <v>0.11494134737017461</v>
+      </c>
+      <c r="D273" s="18">
+        <f>LOG(2000000, 10)</f>
+        <v>6.3010299956639804</v>
+      </c>
+      <c r="E273" s="12">
+        <f>LOG(0.533048009872436, 10)</f>
+        <v>-0.27323367374325269</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A274" s="18">
+        <f>LOG(300000, 10)</f>
+        <v>5.4771212547196617</v>
+      </c>
+      <c r="B274" s="12">
+        <f>LOG(1.9801072359085)</f>
+        <v>0.29668871081820314</v>
+      </c>
+      <c r="D274" s="18">
+        <f>LOG(3000000, 10)</f>
+        <v>6.4771212547196617</v>
+      </c>
+      <c r="E274" s="12">
+        <f>LOG(0.805363392829895, 10)</f>
+        <v>-9.4008114799721459E-2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A275" s="18">
+        <f>LOG(400000, 10)</f>
+        <v>5.6020599913279616</v>
+      </c>
+      <c r="B275" s="12">
+        <f>LOG(2.64833531379699, 10)</f>
+        <v>0.42297297159558589</v>
+      </c>
+      <c r="D275" s="18">
+        <f>LOG(4000000, 10)</f>
+        <v>6.6020599913279616</v>
+      </c>
+      <c r="E275" s="12">
+        <f>LOG(1.06008450984954, 10)</f>
+        <v>2.5340488565087371E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A276" s="18">
+        <f>LOG(500000, 10)</f>
+        <v>5.6989700043360179</v>
+      </c>
+      <c r="B276" s="12">
+        <f>LOG(3.38747413158416, 10)</f>
+        <v>0.52987598740920727</v>
+      </c>
+      <c r="D276" s="18">
+        <f>LOG(5000000, 10)</f>
+        <v>6.6989700043360187</v>
+      </c>
+      <c r="E276" s="12">
+        <f>LOG(1.29993913173675, 10)</f>
+        <v>0.11392301740704261</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A277" s="18">
+        <f>LOG(600000, 10)</f>
+        <v>5.778151250383643</v>
+      </c>
+      <c r="B277" s="12">
+        <f>LOG(4.04164636135101, 10)</f>
+        <v>0.60655831065558008</v>
+      </c>
+      <c r="D277" s="18">
+        <f>LOG(6000000, 10)</f>
+        <v>6.778151250383643</v>
+      </c>
+      <c r="E277" s="12">
+        <f>LOG(1.53579881191253, 10)</f>
+        <v>0.18633432728470342</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A278" s="18">
+        <f>LOG(700000, 10)</f>
+        <v>5.845098040014256</v>
+      </c>
+      <c r="B278" s="12">
+        <f>LOG(4.73281261920928, 10)</f>
+        <v>0.67511931028790428</v>
+      </c>
+      <c r="D278" s="18">
+        <f>LOG(7000000, 10)</f>
+        <v>6.845098040014256</v>
+      </c>
+      <c r="E278" s="12">
+        <f>LOG(1.86769909858703, 10)</f>
+        <v>0.27130690918022438</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A279" s="18">
+        <f>LOG(800000, 10)</f>
+        <v>5.9030899869919429</v>
+      </c>
+      <c r="B279" s="12">
+        <f>LOG(5.41396498680114, 10)</f>
+        <v>0.73351544277393554</v>
+      </c>
+      <c r="D279" s="18">
+        <f>LOG(8000000, 10)</f>
+        <v>6.9030899869919429</v>
+      </c>
+      <c r="E279" s="12">
+        <f>LOG(2.03160903453826, 10)</f>
+        <v>0.30784013546261862</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A280" s="18">
+        <f>LOG(900000, 10)</f>
+        <v>5.9542425094393243</v>
+      </c>
+      <c r="B280" s="12">
+        <f>LOG(6.11122841835022, 10)</f>
+        <v>0.78612851657453708</v>
+      </c>
+      <c r="D280" s="18">
+        <f>LOG(9000000, 10)</f>
+        <v>6.9542425094393234</v>
+      </c>
+      <c r="E280" s="12">
+        <f>LOG(2.41001198291778, 10)</f>
+        <v>0.38201920195334599</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A281" s="18">
+        <f>LOG(1000000, 10)</f>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="B281" s="13">
+        <f>LOG(6.87211816310882, 10)</f>
+        <v>0.83709061839375198</v>
+      </c>
+      <c r="D281" s="18">
+        <f>LOG(10000000, 10)</f>
+        <v>7</v>
+      </c>
+      <c r="E281" s="13">
+        <f>LOG(2.7088038444519, 10)</f>
+        <v>0.43277755713486193</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="D257:E257"/>
+    <mergeCell ref="A270:B270"/>
+    <mergeCell ref="D270:E270"/>
+    <mergeCell ref="B255:D255"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>